<commit_message>
fixed formatting for organizer
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/schedule/Simple-A4.xlsx
+++ b/owlcms/src/main/resources/templates/schedule/Simple-A4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FFCB62-9778-4E2D-AFA3-600EC832762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07921A66-4BAF-4D68-AEEC-0556DC6708C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,9 +624,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -666,6 +663,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,6 +676,15 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,16 +695,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="F2" s="22"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -1240,18 +1240,18 @@
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="23"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="13"/>
       <c r="J3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
       <c r="O3" s="3"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1273,18 +1273,18 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="24"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
       <c r="O4" s="3"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1326,59 +1326,59 @@
         <v>12</v>
       </c>
       <c r="B6" s="34"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="42"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="1:27" s="6" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
       <c r="N7" s="4"/>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
       <c r="N8" s="4"/>
       <c r="O8" s="5"/>
     </row>
@@ -1387,27 +1387,27 @@
         <v>18</v>
       </c>
       <c r="B9" s="35"/>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="38"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -1780,13 +1780,14 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="G9:M9"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:H8">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">

</xml_diff>